<commit_message>
update data + download
</commit_message>
<xml_diff>
--- a/Database/Data_20150722/Class.xlsx
+++ b/Database/Data_20150722/Class.xlsx
@@ -563,14 +563,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>